<commit_message>
Maj du fichier de simulation
</commit_message>
<xml_diff>
--- a/outil-eval-impact-remu.xlsx
+++ b/outil-eval-impact-remu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="28260" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Outil d'évaluation de l'impact des revues de salaire</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Frais de fonctionnement et charges (crédit, loyer, énergie, frais, …)</t>
   </si>
   <si>
-    <t>CA moyen de 180k€ par personne</t>
-  </si>
-  <si>
     <t>Répartition du bénéfice</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>NA - le reste des salariés</t>
   </si>
   <si>
-    <t xml:space="preserve">Salaires fixes + variables </t>
-  </si>
-  <si>
     <t xml:space="preserve">Marge </t>
   </si>
   <si>
@@ -209,17 +203,41 @@
   </si>
   <si>
     <t>Indice INSEE</t>
+  </si>
+  <si>
+    <t>CA moyen par personne</t>
+  </si>
+  <si>
+    <t>Chiffre d'affaire de la société</t>
+  </si>
+  <si>
+    <t>Masse salariale = CA - invest - rem du capital - frais</t>
+  </si>
+  <si>
+    <t>TOTAL ANNUEL</t>
+  </si>
+  <si>
+    <t>Salaires fixes + variables ACTUELS NETS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ [$€-40C]_-;\-* #,##0\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ [$€-40C]_-;\-* #,##0\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_)\ &quot;€&quot;_ ;_ * \(#,##0\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,83 +398,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -468,8 +487,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="32">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -500,6 +520,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Monétaire" xfId="31" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -846,6 +867,7 @@
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="56" customWidth="1"/>
     <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25">
@@ -867,9 +889,12 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6">
-        <f>200*1800000</f>
-        <v>360000000</v>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="6">
+        <f>A6*J4</f>
+        <v>22000000</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -883,7 +908,10 @@
       <c r="D4" s="24"/>
       <c r="E4" s="25"/>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="J4" s="26">
+        <v>110000</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -902,382 +930,408 @@
         <v>200</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="18">
-      <c r="A11" s="3" t="s">
+    <row r="8" spans="1:11" ht="18">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="I11" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="I8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" s="21" customFormat="1" ht="46" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" s="21" customFormat="1" ht="46" customHeight="1">
+      <c r="A9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="B9" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="E9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="G9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="22">
-        <f>I3</f>
-        <v>360000000</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>61</v>
+      <c r="J9" s="22">
+        <f>J3</f>
+        <v>22000000</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <f>(VLOOKUP(B10,'Grille de salaire'!$A$3:$C$15,3,FALSE))</f>
+        <v>2600</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="6">
+        <f>($C10*$D10*12)*$A$4</f>
+        <v>14976</v>
+      </c>
+      <c r="F10">
+        <f>A5</f>
+        <v>200</v>
+      </c>
+      <c r="I10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="6">
+        <f>J9*K10</f>
+        <v>4400000</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(B11,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
+        <v>2600</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" ref="E11:E15" si="0">($C11*$D11*12)*$A$4</f>
+        <v>7488</v>
+      </c>
+      <c r="F11">
+        <f>A5</f>
+        <v>200</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="6">
+        <f>J10/3</f>
+        <v>1466666.6666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(B12,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
+        <v>6100</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>A5/2</f>
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="6">
+        <f>J10/3</f>
+        <v>1466666.6666666667</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C13">
-        <f>(VLOOKUP(B13,'Grille de salaire'!$A$3:$C$15,3,FALSE))</f>
-        <v>2600</v>
+        <f>VLOOKUP(B13,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
+        <v>6100</v>
       </c>
       <c r="D13" s="8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="6">
-        <f>($C13*$D13*12)*$A$4</f>
-        <v>14976</v>
+        <f t="shared" si="0"/>
+        <v>43920</v>
       </c>
       <c r="F13">
         <f>A5</f>
         <v>200</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J13" s="6">
-        <f>J12*K13</f>
-        <v>72000000</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0.2</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <f>VLOOKUP(B14,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
-        <v>2600</v>
+        <v>2100</v>
       </c>
       <c r="D14" s="8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" ref="E14:E18" si="0">($C14*$D14*12)*$A$4</f>
-        <v>7488</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F14">
         <f>A5</f>
         <v>200</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="J14" s="6">
-        <v>20000000</v>
+        <f>12*C17+E17</f>
+        <v>11618352</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <f>VLOOKUP(B15,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
-        <v>6100</v>
+        <v>4100</v>
       </c>
       <c r="D15" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5904</v>
       </c>
       <c r="F15">
-        <f>A5/2</f>
-        <v>100</v>
+        <f>A5</f>
+        <v>200</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J15" s="6">
-        <f>10%*J12</f>
-        <v>36000000</v>
+        <f>C18*(1+0.5+0.24)</f>
+        <v>17100720</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
       </c>
       <c r="C16">
-        <f>VLOOKUP(B16,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
-        <v>6100</v>
+        <v>4100</v>
       </c>
       <c r="D16" s="8">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="0"/>
-        <v>43920</v>
+        <f>($C16*$D16*12)*$A$4*(A6-COUNTA(B10:B15))</f>
+        <v>1718064</v>
       </c>
       <c r="F16">
-        <f>A5</f>
-        <v>200</v>
+        <f>A5*(A6-COUNTA(A10:A15))</f>
+        <v>38800</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="J16" s="6">
-        <v>120000000</v>
+        <f>J9-J11-J12-J13</f>
+        <v>17866666.666666664</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
       <c r="B17" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C17">
-        <f>VLOOKUP(B17,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
-        <v>2100</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0</v>
+        <f>SUM(C10:C15)+C16*(A6-COUNTA(A10:A15))</f>
+        <v>819000</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:E17" si="1">SUM(D10:D16)</f>
+        <v>1.35</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f>A5</f>
-        <v>200</v>
-      </c>
-      <c r="I17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="6">
-        <f>J18*(1+0.5+0.24)</f>
-        <v>116846715.32846715</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <f>VLOOKUP(B18,'Grille de salaire'!$A$3:$C$15,3,FALSE)</f>
-        <v>4100</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="6">
-        <f t="shared" si="0"/>
-        <v>5904</v>
-      </c>
-      <c r="F18">
-        <f>A5</f>
-        <v>200</v>
-      </c>
-      <c r="I18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="6">
-        <f>(J12-SUM(J14:J16))/2.74</f>
-        <v>67153284.67153284</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19">
-        <v>4100</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="E19" s="6">
-        <f>($C19*$D19*12)*$A$4*(A6-COUNTA(B13:B18))</f>
-        <v>1718064</v>
-      </c>
-      <c r="F19">
-        <f>A5*(A6-COUNTA(A13:A18))</f>
-        <v>38800</v>
-      </c>
-      <c r="I19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="6">
-        <f>12*C20+E20</f>
-        <v>11618352</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="B20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20">
-        <f>SUM(C13:C18)+C19*(A6-COUNTA(A13:A18))</f>
-        <v>819000</v>
-      </c>
-      <c r="D20">
-        <f t="shared" ref="D20:E20" si="1">SUM(D13:D19)</f>
-        <v>1.35</v>
-      </c>
-      <c r="E20" s="6">
         <f t="shared" si="1"/>
         <v>1790352</v>
       </c>
-      <c r="F20">
-        <f>SUM(F13:F19)</f>
+      <c r="F17">
+        <f>SUM(F10:F16)</f>
         <v>39900</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="18">
-      <c r="A22" s="5" t="s">
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="6">
+        <f>(J9-SUM(J11:J13))/2.74</f>
+        <v>6520681.2652068129</v>
+      </c>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18">
+        <f>C17*12</f>
+        <v>9828000</v>
+      </c>
+      <c r="E18" s="6">
+        <f>E17</f>
+        <v>1790352</v>
+      </c>
+      <c r="F18" s="6">
+        <f>E18+C18</f>
+        <v>11618352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18">
+      <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="5">
         <v>1.02</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="I22" s="5" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="I19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="6">
+        <v>360000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="6">
+        <f>J20*K21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="6">
+        <v>200000</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J23" s="6">
-        <v>360000000</v>
+        <f>5%*J20</f>
+        <v>18000000</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
       <c r="I24" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J24" s="6">
-        <f>J23*K24</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="8">
-        <v>0</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
       <c r="I25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J25" s="6">
-        <v>200000</v>
+        <f>J26*(1+0.5+0.24)</f>
+        <v>216293430.65693429</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J26" s="6">
-        <f>5%*J23</f>
-        <v>18000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="I27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="6">
-        <v>1200000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="I28" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" s="6">
-        <f>J29*(1+0.5+0.24)</f>
-        <v>216293430.65693429</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="I29" t="s">
-        <v>40</v>
-      </c>
-      <c r="J29" s="6">
-        <f>(J23-SUM(J25:J27))/2.74</f>
+        <f>(J20-SUM(J22:J24))/2.74</f>
         <v>124306569.34306568</v>
       </c>
     </row>
@@ -1318,10 +1372,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -1344,7 +1398,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>16</v>

</xml_diff>